<commit_message>
Fix RunTimeWarning caused by having all nan values in CM sigma array for probability of detection
</commit_message>
<xml_diff>
--- a/00_raw_reports/Kairos_Stage1_submitted-2022-11-17.xlsx
+++ b/00_raw_reports/Kairos_Stage1_submitted-2022-11-17.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E73C7EE-A0DA-AF46-8E37-3F8410CDD406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7D86B1-4EE1-7C41-8205-A79F14FE0AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -1412,7 +1412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S528"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E12" sqref="E12"/>
       <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
@@ -24273,7 +24273,7 @@
   <dimension ref="A1:S528"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E12" sqref="E12"/>
       <selection pane="bottomLeft" activeCell="K228" sqref="K228"/>
     </sheetView>

</xml_diff>